<commit_message>
Foram preenchidos os dados do ficheiro excel. Falta acabar o undersample do variance threshold
</commit_message>
<xml_diff>
--- a/Trabalho_Pratico/Fase_2/Model Comparison.xlsx
+++ b/Trabalho_Pratico/Fase_2/Model Comparison.xlsx
@@ -5,15 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Eu\ISEL\MEIC\2_Semestre\MDLE-23-24\Trabalho_Pratico\Fase_2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ricardo\Github\MDLE-23-24\Trabalho_Pratico\Fase_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52BE84A3-ED67-4CA5-9729-87BBF58C94CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE3ED7BA-F120-416F-A228-114686DB4590}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Folha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Energy Dataset" sheetId="1" r:id="rId1"/>
+    <sheet name="Weather Dataset" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="62">
   <si>
     <t>Energy Dataset</t>
   </si>
@@ -70,6 +71,147 @@
   </si>
   <si>
     <t>Com o dataset da Feature Selection</t>
+  </si>
+  <si>
+    <t>Dataset com Fisher's Ratio</t>
+  </si>
+  <si>
+    <t>Conditions</t>
+  </si>
+  <si>
+    <t>Instances</t>
+  </si>
+  <si>
+    <t>Information Gain Training</t>
+  </si>
+  <si>
+    <t>Fisher's Ratio Training</t>
+  </si>
+  <si>
+    <t>Fisher's Ratio Test</t>
+  </si>
+  <si>
+    <t>Information Gain Test</t>
+  </si>
+  <si>
+    <t>Variance Threshold Training</t>
+  </si>
+  <si>
+    <t>Variance Threshold Test</t>
+  </si>
+  <si>
+    <t>rmse</t>
+  </si>
+  <si>
+    <t>mse</t>
+  </si>
+  <si>
+    <t>r2</t>
+  </si>
+  <si>
+    <t>mae</t>
+  </si>
+  <si>
+    <t>Dataset com Information Gain</t>
+  </si>
+  <si>
+    <t>0.362</t>
+  </si>
+  <si>
+    <t>0.131</t>
+  </si>
+  <si>
+    <t>0.832</t>
+  </si>
+  <si>
+    <t>0.22</t>
+  </si>
+  <si>
+    <t>0.308</t>
+  </si>
+  <si>
+    <t>0.095</t>
+  </si>
+  <si>
+    <t>0.883</t>
+  </si>
+  <si>
+    <t>0.195</t>
+  </si>
+  <si>
+    <t>0.356</t>
+  </si>
+  <si>
+    <t>0.127</t>
+  </si>
+  <si>
+    <t>0.846</t>
+  </si>
+  <si>
+    <t>0.225</t>
+  </si>
+  <si>
+    <t>0.455</t>
+  </si>
+  <si>
+    <t>0.207</t>
+  </si>
+  <si>
+    <t>0.734</t>
+  </si>
+  <si>
+    <t>0.368</t>
+  </si>
+  <si>
+    <t>0.373</t>
+  </si>
+  <si>
+    <t>0.139</t>
+  </si>
+  <si>
+    <t>0.829</t>
+  </si>
+  <si>
+    <t>0.269</t>
+  </si>
+  <si>
+    <t>Dataset com Variance Threshold</t>
+  </si>
+  <si>
+    <t>0.439</t>
+  </si>
+  <si>
+    <t>0.193</t>
+  </si>
+  <si>
+    <t>0.766</t>
+  </si>
+  <si>
+    <t>0.347</t>
+  </si>
+  <si>
+    <t>0.535</t>
+  </si>
+  <si>
+    <t>0.286</t>
+  </si>
+  <si>
+    <t>0.632</t>
+  </si>
+  <si>
+    <t>0.445</t>
+  </si>
+  <si>
+    <t>0.578</t>
+  </si>
+  <si>
+    <t>0.334</t>
+  </si>
+  <si>
+    <t>0.589</t>
+  </si>
+  <si>
+    <t>0.514</t>
   </si>
 </sst>
 </file>
@@ -99,9 +241,46 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
@@ -111,12 +290,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -399,8 +592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -432,12 +625,12 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
@@ -466,7 +659,7 @@
       <c r="D7">
         <v>7.6999999999999999E-2</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="1" t="s">
         <v>13</v>
       </c>
     </row>
@@ -483,7 +676,7 @@
       <c r="D8">
         <v>0.96199999999999997</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="1" t="s">
         <v>13</v>
       </c>
     </row>
@@ -500,7 +693,7 @@
       <c r="D9">
         <v>0.92</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="1" t="s">
         <v>13</v>
       </c>
     </row>
@@ -517,7 +710,7 @@
       <c r="D10">
         <v>0.92300000000000004</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="1" t="s">
         <v>13</v>
       </c>
     </row>
@@ -534,17 +727,17 @@
       <c r="D11">
         <v>0.98799999999999999</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
@@ -573,7 +766,7 @@
       <c r="D16">
         <v>1E-3</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E16" s="1" t="s">
         <v>13</v>
       </c>
     </row>
@@ -590,7 +783,7 @@
       <c r="D17">
         <v>0.71599999999999997</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E17" s="1" t="s">
         <v>13</v>
       </c>
     </row>
@@ -607,7 +800,7 @@
       <c r="D18">
         <v>0.47</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="E18" s="1" t="s">
         <v>13</v>
       </c>
     </row>
@@ -624,7 +817,7 @@
       <c r="D19">
         <v>0.999</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="E19" s="1" t="s">
         <v>13</v>
       </c>
     </row>
@@ -641,7 +834,7 @@
       <c r="D20">
         <v>0.52300000000000002</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="E20" s="1" t="s">
         <v>13</v>
       </c>
     </row>
@@ -652,4 +845,513 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF879E42-A152-498B-9F7D-3EABAA260A27}">
+  <dimension ref="A3:O25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" customWidth="1"/>
+    <col min="9" max="9" width="11.5703125" customWidth="1"/>
+    <col min="11" max="11" width="14" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" customWidth="1"/>
+    <col min="14" max="14" width="13" customWidth="1"/>
+    <col min="15" max="15" width="13.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="3"/>
+      <c r="K3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L3" s="3"/>
+      <c r="N3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="O3" s="3"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="7"/>
+      <c r="B4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="H4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="7"/>
+      <c r="B5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" s="4">
+        <v>1</v>
+      </c>
+      <c r="I5" s="4">
+        <v>1189</v>
+      </c>
+      <c r="K5" s="4">
+        <v>1</v>
+      </c>
+      <c r="L5" s="4">
+        <v>1146</v>
+      </c>
+      <c r="N5" s="4">
+        <v>1</v>
+      </c>
+      <c r="O5" s="4">
+        <v>1150</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="H6" s="4">
+        <v>2</v>
+      </c>
+      <c r="I6" s="4">
+        <v>278</v>
+      </c>
+      <c r="K6" s="4">
+        <v>2</v>
+      </c>
+      <c r="L6" s="4">
+        <v>297</v>
+      </c>
+      <c r="N6" s="4">
+        <v>2</v>
+      </c>
+      <c r="O6" s="4">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H7" s="4">
+        <v>3</v>
+      </c>
+      <c r="I7" s="4">
+        <v>3292</v>
+      </c>
+      <c r="K7" s="4">
+        <v>3</v>
+      </c>
+      <c r="L7" s="4">
+        <v>3319</v>
+      </c>
+      <c r="N7" s="4">
+        <v>3</v>
+      </c>
+      <c r="O7" s="4">
+        <v>3326</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="H8" s="4">
+        <v>4</v>
+      </c>
+      <c r="I8" s="4">
+        <v>10</v>
+      </c>
+      <c r="K8" s="4">
+        <v>4</v>
+      </c>
+      <c r="L8" s="4">
+        <v>6</v>
+      </c>
+      <c r="N8" s="4">
+        <v>4</v>
+      </c>
+      <c r="O8" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="H9" s="4">
+        <v>5</v>
+      </c>
+      <c r="I9" s="4">
+        <v>52</v>
+      </c>
+      <c r="K9" s="4">
+        <v>5</v>
+      </c>
+      <c r="L9" s="4">
+        <v>53</v>
+      </c>
+      <c r="N9" s="4">
+        <v>5</v>
+      </c>
+      <c r="O9" s="4">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="5"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="7"/>
+      <c r="B12" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="H12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I12" s="3"/>
+      <c r="K12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L12" s="3"/>
+      <c r="N12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="O12" s="3"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="6"/>
+      <c r="B13" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="N13" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="O13" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14" s="8"/>
+      <c r="H14" s="4">
+        <v>1</v>
+      </c>
+      <c r="I14" s="4">
+        <v>580</v>
+      </c>
+      <c r="K14" s="4">
+        <v>1</v>
+      </c>
+      <c r="L14" s="4">
+        <v>623</v>
+      </c>
+      <c r="N14" s="4">
+        <v>1</v>
+      </c>
+      <c r="O14" s="4">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="H15" s="4">
+        <v>2</v>
+      </c>
+      <c r="I15" s="4">
+        <v>170</v>
+      </c>
+      <c r="K15" s="4">
+        <v>2</v>
+      </c>
+      <c r="L15" s="4">
+        <v>151</v>
+      </c>
+      <c r="N15" s="4">
+        <v>2</v>
+      </c>
+      <c r="O15" s="4">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="H16" s="4">
+        <v>3</v>
+      </c>
+      <c r="I16" s="4">
+        <v>1698</v>
+      </c>
+      <c r="K16" s="4">
+        <v>3</v>
+      </c>
+      <c r="L16" s="4">
+        <v>1671</v>
+      </c>
+      <c r="N16" s="4">
+        <v>3</v>
+      </c>
+      <c r="O16" s="4">
+        <v>1664</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="H17" s="4">
+        <v>4</v>
+      </c>
+      <c r="I17" s="4">
+        <v>2</v>
+      </c>
+      <c r="K17" s="4">
+        <v>4</v>
+      </c>
+      <c r="L17" s="4">
+        <v>6</v>
+      </c>
+      <c r="N17" s="4">
+        <v>4</v>
+      </c>
+      <c r="O17" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F18" s="5"/>
+      <c r="H18" s="4">
+        <v>5</v>
+      </c>
+      <c r="I18" s="4">
+        <v>24</v>
+      </c>
+      <c r="K18" s="4">
+        <v>5</v>
+      </c>
+      <c r="L18" s="4">
+        <v>23</v>
+      </c>
+      <c r="N18" s="4">
+        <v>5</v>
+      </c>
+      <c r="O18" s="4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="5"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="7"/>
+      <c r="B20" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="7"/>
+      <c r="B21" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D22" s="4"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D23" s="4"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D24" s="4"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D25" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="N12:O12"/>
+    <mergeCell ref="B12:D12"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Foi adicionado o F1 score, falta o auROC
</commit_message>
<xml_diff>
--- a/Trabalho_Pratico/Fase_2/Model Comparison.xlsx
+++ b/Trabalho_Pratico/Fase_2/Model Comparison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ricardo\Github\MDLE-23-24\Trabalho_Pratico\Fase_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE3ED7BA-F120-416F-A228-114686DB4590}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEC5E9AD-5513-406C-A7B0-9AD2AB944C95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Energy Dataset" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="64">
   <si>
     <t>Energy Dataset</t>
   </si>
@@ -212,6 +212,12 @@
   </si>
   <si>
     <t>0.514</t>
+  </si>
+  <si>
+    <t>F1 Score</t>
+  </si>
+  <si>
+    <t>Area under ROC</t>
   </si>
 </sst>
 </file>
@@ -290,26 +296,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -590,10 +595,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:E20"/>
+  <dimension ref="A2:E23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -625,12 +630,12 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
@@ -731,57 +736,65 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="2" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12">
+        <v>0.86399999999999999</v>
+      </c>
+      <c r="C12">
+        <v>0.95099999999999996</v>
+      </c>
+      <c r="D12">
+        <v>0.95199999999999996</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>63</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
         <v>1</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C16" t="s">
         <v>3</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D16" t="s">
         <v>4</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E16" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16">
-        <v>2E-3</v>
-      </c>
-      <c r="C16">
-        <v>0.01</v>
-      </c>
-      <c r="D16">
-        <v>1E-3</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B17">
-        <v>0.8</v>
+        <v>2E-3</v>
       </c>
       <c r="C17">
-        <v>0.71599999999999997</v>
+        <v>0.01</v>
       </c>
       <c r="D17">
-        <v>0.71599999999999997</v>
+        <v>1E-3</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>13</v>
@@ -789,16 +802,16 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B18">
-        <v>0.61499999999999999</v>
+        <v>0.8</v>
       </c>
       <c r="C18">
-        <v>0.47</v>
+        <v>0.71599999999999997</v>
       </c>
       <c r="D18">
-        <v>0.47</v>
+        <v>0.71599999999999997</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>13</v>
@@ -806,16 +819,16 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B19">
-        <v>0.998</v>
+        <v>0.61499999999999999</v>
       </c>
       <c r="C19">
-        <v>0.999</v>
+        <v>0.47</v>
       </c>
       <c r="D19">
-        <v>0.999</v>
+        <v>0.47</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>13</v>
@@ -823,25 +836,67 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20">
+        <v>0.998</v>
+      </c>
+      <c r="C20">
+        <v>0.999</v>
+      </c>
+      <c r="D20">
+        <v>0.999</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>12</v>
       </c>
-      <c r="B20">
+      <c r="B21">
         <v>0.66400000000000003</v>
       </c>
-      <c r="C20">
+      <c r="C21">
         <v>0.52300000000000002</v>
       </c>
-      <c r="D20">
+      <c r="D21">
         <v>0.52300000000000002</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E21" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>62</v>
+      </c>
+      <c r="B22">
+        <v>0.80200000000000005</v>
+      </c>
+      <c r="C22">
+        <v>0.74</v>
+      </c>
+      <c r="D22">
+        <v>0.74</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>63</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B15:E15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -851,7 +906,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF879E42-A152-498B-9F7D-3EABAA260A27}">
   <dimension ref="A3:O25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
@@ -869,488 +924,481 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="3"/>
-      <c r="K3" s="3" t="s">
+      <c r="I3" s="7"/>
+      <c r="K3" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="L3" s="3"/>
-      <c r="N3" s="3" t="s">
+      <c r="L3" s="7"/>
+      <c r="N3" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="O3" s="3"/>
+      <c r="O3" s="7"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
-      <c r="B4" s="3" t="s">
+      <c r="A4" s="4"/>
+      <c r="B4" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="H4" s="4" t="s">
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="H4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="K4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="4" t="s">
+      <c r="L4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="N4" s="4" t="s">
+      <c r="N4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="O4" s="4" t="s">
+      <c r="O4" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="4" t="s">
+      <c r="A5" s="4"/>
+      <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5" s="2">
         <v>1</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="2">
         <v>1189</v>
       </c>
-      <c r="K5" s="4">
+      <c r="K5" s="2">
         <v>1</v>
       </c>
-      <c r="L5" s="4">
+      <c r="L5" s="2">
         <v>1146</v>
       </c>
-      <c r="N5" s="4">
+      <c r="N5" s="2">
         <v>1</v>
       </c>
-      <c r="O5" s="4">
+      <c r="O5" s="2">
         <v>1150</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6" s="2">
         <v>2</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6" s="2">
         <v>278</v>
       </c>
-      <c r="K6" s="4">
+      <c r="K6" s="2">
         <v>2</v>
       </c>
-      <c r="L6" s="4">
+      <c r="L6" s="2">
         <v>297</v>
       </c>
-      <c r="N6" s="4">
+      <c r="N6" s="2">
         <v>2</v>
       </c>
-      <c r="O6" s="4">
+      <c r="O6" s="2">
         <v>291</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7" s="2">
         <v>3</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7" s="2">
         <v>3292</v>
       </c>
-      <c r="K7" s="4">
+      <c r="K7" s="2">
         <v>3</v>
       </c>
-      <c r="L7" s="4">
+      <c r="L7" s="2">
         <v>3319</v>
       </c>
-      <c r="N7" s="4">
+      <c r="N7" s="2">
         <v>3</v>
       </c>
-      <c r="O7" s="4">
+      <c r="O7" s="2">
         <v>3326</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H8" s="2">
         <v>4</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I8" s="2">
         <v>10</v>
       </c>
-      <c r="K8" s="4">
+      <c r="K8" s="2">
         <v>4</v>
       </c>
-      <c r="L8" s="4">
+      <c r="L8" s="2">
         <v>6</v>
       </c>
-      <c r="N8" s="4">
+      <c r="N8" s="2">
         <v>4</v>
       </c>
-      <c r="O8" s="4">
+      <c r="O8" s="2">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="H9" s="4">
+      <c r="H9" s="2">
         <v>5</v>
       </c>
-      <c r="I9" s="4">
+      <c r="I9" s="2">
         <v>52</v>
       </c>
-      <c r="K9" s="4">
+      <c r="K9" s="2">
         <v>5</v>
       </c>
-      <c r="L9" s="4">
+      <c r="L9" s="2">
         <v>53</v>
       </c>
-      <c r="N9" s="4">
+      <c r="N9" s="2">
         <v>5</v>
       </c>
-      <c r="O9" s="4">
+      <c r="O9" s="2">
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-    </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="3" t="s">
+      <c r="A12" s="4"/>
+      <c r="B12" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="H12" s="3" t="s">
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="H12" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="I12" s="3"/>
-      <c r="K12" s="3" t="s">
+      <c r="I12" s="7"/>
+      <c r="K12" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="L12" s="3"/>
-      <c r="N12" s="3" t="s">
+      <c r="L12" s="7"/>
+      <c r="N12" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="O12" s="3"/>
+      <c r="O12" s="7"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
-      <c r="B13" s="4" t="s">
+      <c r="A13" s="3"/>
+      <c r="B13" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H13" s="4" t="s">
+      <c r="H13" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I13" s="4" t="s">
+      <c r="I13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="K13" s="4" t="s">
+      <c r="K13" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="L13" s="4" t="s">
+      <c r="L13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="N13" s="4" t="s">
+      <c r="N13" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="O13" s="4" t="s">
+      <c r="O13" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E14" s="8"/>
-      <c r="H14" s="4">
+      <c r="E14" s="5"/>
+      <c r="H14" s="2">
         <v>1</v>
       </c>
-      <c r="I14" s="4">
+      <c r="I14" s="2">
         <v>580</v>
       </c>
-      <c r="K14" s="4">
+      <c r="K14" s="2">
         <v>1</v>
       </c>
-      <c r="L14" s="4">
+      <c r="L14" s="2">
         <v>623</v>
       </c>
-      <c r="N14" s="4">
+      <c r="N14" s="2">
         <v>1</v>
       </c>
-      <c r="O14" s="4">
+      <c r="O14" s="2">
         <v>619</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="H15" s="4">
+      <c r="H15" s="2">
         <v>2</v>
       </c>
-      <c r="I15" s="4">
+      <c r="I15" s="2">
         <v>170</v>
       </c>
-      <c r="K15" s="4">
+      <c r="K15" s="2">
         <v>2</v>
       </c>
-      <c r="L15" s="4">
+      <c r="L15" s="2">
         <v>151</v>
       </c>
-      <c r="N15" s="4">
+      <c r="N15" s="2">
         <v>2</v>
       </c>
-      <c r="O15" s="4">
+      <c r="O15" s="2">
         <v>157</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="H16" s="4">
+      <c r="H16" s="2">
         <v>3</v>
       </c>
-      <c r="I16" s="4">
+      <c r="I16" s="2">
         <v>1698</v>
       </c>
-      <c r="K16" s="4">
+      <c r="K16" s="2">
         <v>3</v>
       </c>
-      <c r="L16" s="4">
+      <c r="L16" s="2">
         <v>1671</v>
       </c>
-      <c r="N16" s="4">
+      <c r="N16" s="2">
         <v>3</v>
       </c>
-      <c r="O16" s="4">
+      <c r="O16" s="2">
         <v>1664</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="H17" s="4">
+      <c r="H17" s="2">
         <v>4</v>
       </c>
-      <c r="I17" s="4">
+      <c r="I17" s="2">
         <v>2</v>
       </c>
-      <c r="K17" s="4">
+      <c r="K17" s="2">
         <v>4</v>
       </c>
-      <c r="L17" s="4">
+      <c r="L17" s="2">
         <v>6</v>
       </c>
-      <c r="N17" s="4">
+      <c r="N17" s="2">
         <v>4</v>
       </c>
-      <c r="O17" s="4">
+      <c r="O17" s="2">
         <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F18" s="5"/>
-      <c r="H18" s="4">
+      <c r="H18" s="2">
         <v>5</v>
       </c>
-      <c r="I18" s="4">
+      <c r="I18" s="2">
         <v>24</v>
       </c>
-      <c r="K18" s="4">
+      <c r="K18" s="2">
         <v>5</v>
       </c>
-      <c r="L18" s="4">
+      <c r="L18" s="2">
         <v>23</v>
       </c>
-      <c r="N18" s="4">
+      <c r="N18" s="2">
         <v>5</v>
       </c>
-      <c r="O18" s="4">
+      <c r="O18" s="2">
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
-    </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
-      <c r="B20" s="3" t="s">
+      <c r="A20" s="4"/>
+      <c r="B20" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
-      <c r="B21" s="4" t="s">
+      <c r="A21" s="4"/>
+      <c r="B21" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D21" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D22" s="4"/>
+      <c r="D22" s="2"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D23" s="4"/>
+      <c r="D23" s="2"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D24" s="4"/>
+      <c r="D24" s="2"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
+      <c r="A25" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D25" s="4"/>
+      <c r="D25" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="N12:O12"/>
+    <mergeCell ref="B12:D12"/>
     <mergeCell ref="B20:D20"/>
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="H3:I3"/>
     <mergeCell ref="H12:I12"/>
     <mergeCell ref="K3:L3"/>
     <mergeCell ref="K12:L12"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="N12:O12"/>
-    <mergeCell ref="B12:D12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Foi adicionado o cálculo do auc
</commit_message>
<xml_diff>
--- a/Trabalho_Pratico/Fase_2/Model Comparison.xlsx
+++ b/Trabalho_Pratico/Fase_2/Model Comparison.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ricardo\Github\MDLE-23-24\Trabalho_Pratico\Fase_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEC5E9AD-5513-406C-A7B0-9AD2AB944C95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8A0B867-693E-4948-A2FD-C5B9C0CD3BD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -597,8 +597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -757,6 +757,15 @@
       <c r="A13" t="s">
         <v>63</v>
       </c>
+      <c r="B13">
+        <v>0.88100000000000001</v>
+      </c>
+      <c r="C13">
+        <v>0.95699999999999996</v>
+      </c>
+      <c r="D13">
+        <v>0.95599999999999996</v>
+      </c>
       <c r="E13" s="1" t="s">
         <v>13</v>
       </c>
@@ -888,6 +897,15 @@
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>63</v>
+      </c>
+      <c r="B23">
+        <v>0.83099999999999996</v>
+      </c>
+      <c r="C23">
+        <v>0.76100000000000001</v>
+      </c>
+      <c r="D23">
+        <v>0.76100000000000001</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Adicionei modelos ao energy, adicionei comparação de modelos
</commit_message>
<xml_diff>
--- a/Trabalho_Pratico/Fase_2/Model Comparison.xlsx
+++ b/Trabalho_Pratico/Fase_2/Model Comparison.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rreis\Desktop\MEIC\2_Semestre\MDLE-23-24\Trabalho_Pratico\Fase_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31C3BF89-300B-427C-A44F-1EBB7CF0472B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7882AD2-5A6E-49EC-A821-91F694E4094F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Energy Dataset" sheetId="1" r:id="rId1"/>
-    <sheet name="Weather Dataset" sheetId="2" r:id="rId2"/>
+    <sheet name="Energy Dataset Models" sheetId="3" r:id="rId2"/>
+    <sheet name="Weather Dataset" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="73">
   <si>
     <t>Energy Dataset</t>
   </si>
@@ -227,6 +228,24 @@
   </si>
   <si>
     <t>SEED = 321</t>
+  </si>
+  <si>
+    <t>SEED = 1111</t>
+  </si>
+  <si>
+    <t>SEED = 377</t>
+  </si>
+  <si>
+    <t>Random Forest</t>
+  </si>
+  <si>
+    <t>Logistic Regression</t>
+  </si>
+  <si>
+    <t>Decision Trees</t>
+  </si>
+  <si>
+    <t>SEED = 333</t>
   </si>
 </sst>
 </file>
@@ -242,7 +261,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -252,6 +271,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -305,7 +330,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -319,6 +344,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -606,8 +634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:R23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -756,12 +784,6 @@
       <c r="O7">
         <v>0.126</v>
       </c>
-      <c r="P7">
-        <v>6.8000000000000005E-2</v>
-      </c>
-      <c r="Q7">
-        <v>7.0000000000000007E-2</v>
-      </c>
       <c r="R7" s="1" t="s">
         <v>13</v>
       </c>
@@ -803,12 +825,6 @@
       <c r="O8">
         <v>0.94199999999999995</v>
       </c>
-      <c r="P8">
-        <v>0.96199999999999997</v>
-      </c>
-      <c r="Q8">
-        <v>0.96099999999999997</v>
-      </c>
       <c r="R8" s="1" t="s">
         <v>13</v>
       </c>
@@ -850,12 +866,6 @@
       <c r="O9">
         <v>0.878</v>
       </c>
-      <c r="P9">
-        <v>0.92</v>
-      </c>
-      <c r="Q9">
-        <v>0.91800000000000004</v>
-      </c>
       <c r="R9" s="1" t="s">
         <v>13</v>
       </c>
@@ -897,12 +907,6 @@
       <c r="O10">
         <v>0.874</v>
       </c>
-      <c r="P10">
-        <v>0.93200000000000005</v>
-      </c>
-      <c r="Q10">
-        <v>0.93</v>
-      </c>
       <c r="R10" s="1" t="s">
         <v>13</v>
       </c>
@@ -944,12 +948,6 @@
       <c r="O11">
         <v>0.98899999999999999</v>
       </c>
-      <c r="P11">
-        <v>0.98099999999999998</v>
-      </c>
-      <c r="Q11">
-        <v>0.98199999999999998</v>
-      </c>
       <c r="R11" s="1" t="s">
         <v>13</v>
       </c>
@@ -991,12 +989,6 @@
       <c r="O12">
         <v>0.92400000000000004</v>
       </c>
-      <c r="P12">
-        <v>0.95099999999999996</v>
-      </c>
-      <c r="Q12">
-        <v>0.95</v>
-      </c>
       <c r="R12" s="1" t="s">
         <v>13</v>
       </c>
@@ -1037,12 +1029,6 @@
       </c>
       <c r="O13">
         <v>0.93100000000000005</v>
-      </c>
-      <c r="P13">
-        <v>0.95699999999999996</v>
-      </c>
-      <c r="Q13">
-        <v>0.95599999999999996</v>
       </c>
       <c r="R13" s="1" t="s">
         <v>13</v>
@@ -1061,6 +1047,12 @@
       <c r="J15" s="6"/>
       <c r="K15" s="6"/>
       <c r="L15" s="6"/>
+      <c r="O15" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="P15" s="6"/>
+      <c r="Q15" s="6"/>
+      <c r="R15" s="6"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
@@ -1087,8 +1079,20 @@
       <c r="L16" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O16" t="s">
+        <v>1</v>
+      </c>
+      <c r="P16" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>4</v>
+      </c>
+      <c r="R16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -1107,11 +1111,35 @@
       <c r="H17" t="s">
         <v>8</v>
       </c>
+      <c r="I17">
+        <v>0.14599999999999999</v>
+      </c>
+      <c r="J17">
+        <v>1E-3</v>
+      </c>
+      <c r="K17">
+        <v>1E-3</v>
+      </c>
       <c r="L17" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N17" t="s">
+        <v>8</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17">
+        <v>1E-3</v>
+      </c>
+      <c r="Q17">
+        <v>1E-3</v>
+      </c>
+      <c r="R17" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>9</v>
       </c>
@@ -1130,11 +1158,35 @@
       <c r="H18" t="s">
         <v>9</v>
       </c>
+      <c r="I18">
+        <v>0.73799999999999999</v>
+      </c>
+      <c r="J18">
+        <v>0.71499999999999997</v>
+      </c>
+      <c r="K18">
+        <v>0.71499999999999997</v>
+      </c>
       <c r="L18" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N18" t="s">
+        <v>9</v>
+      </c>
+      <c r="O18">
+        <v>0.747</v>
+      </c>
+      <c r="P18">
+        <v>0.71699999999999997</v>
+      </c>
+      <c r="Q18">
+        <v>0.71699999999999997</v>
+      </c>
+      <c r="R18" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>10</v>
       </c>
@@ -1153,11 +1205,35 @@
       <c r="H19" t="s">
         <v>10</v>
       </c>
+      <c r="I19">
+        <v>0.48499999999999999</v>
+      </c>
+      <c r="J19">
+        <v>0.46899999999999997</v>
+      </c>
+      <c r="K19">
+        <v>0.46899999999999997</v>
+      </c>
       <c r="L19" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N19" t="s">
+        <v>10</v>
+      </c>
+      <c r="O19">
+        <v>0.52300000000000002</v>
+      </c>
+      <c r="P19">
+        <v>0.47199999999999998</v>
+      </c>
+      <c r="Q19">
+        <v>0.47199999999999998</v>
+      </c>
+      <c r="R19" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>11</v>
       </c>
@@ -1176,11 +1252,35 @@
       <c r="H20" t="s">
         <v>11</v>
       </c>
+      <c r="I20">
+        <v>0.85399999999999998</v>
+      </c>
+      <c r="J20">
+        <v>0.999</v>
+      </c>
+      <c r="K20">
+        <v>0.999</v>
+      </c>
       <c r="L20" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N20" t="s">
+        <v>11</v>
+      </c>
+      <c r="O20">
+        <v>1</v>
+      </c>
+      <c r="P20">
+        <v>0.999</v>
+      </c>
+      <c r="Q20">
+        <v>0.999</v>
+      </c>
+      <c r="R20" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -1199,11 +1299,35 @@
       <c r="H21" t="s">
         <v>12</v>
       </c>
+      <c r="I21">
+        <v>0.65800000000000003</v>
+      </c>
+      <c r="J21">
+        <v>0.52100000000000002</v>
+      </c>
+      <c r="K21">
+        <v>0.52100000000000002</v>
+      </c>
       <c r="L21" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N21" t="s">
+        <v>12</v>
+      </c>
+      <c r="O21">
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="P21">
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="Q21">
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="R21" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>62</v>
       </c>
@@ -1222,11 +1346,35 @@
       <c r="H22" t="s">
         <v>62</v>
       </c>
+      <c r="I22">
+        <v>0.72599999999999998</v>
+      </c>
+      <c r="J22">
+        <v>0.74</v>
+      </c>
+      <c r="K22">
+        <v>0.74</v>
+      </c>
       <c r="L22" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N22" t="s">
+        <v>62</v>
+      </c>
+      <c r="O22">
+        <v>0.76200000000000001</v>
+      </c>
+      <c r="P22">
+        <v>0.74099999999999999</v>
+      </c>
+      <c r="Q22">
+        <v>0.74099999999999999</v>
+      </c>
+      <c r="R22" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>63</v>
       </c>
@@ -1245,12 +1393,36 @@
       <c r="H23" t="s">
         <v>63</v>
       </c>
+      <c r="I23">
+        <v>0.77600000000000002</v>
+      </c>
+      <c r="J23">
+        <v>0.76</v>
+      </c>
+      <c r="K23">
+        <v>0.76100000000000001</v>
+      </c>
       <c r="L23" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="N23" t="s">
+        <v>63</v>
+      </c>
+      <c r="O23">
+        <v>0.78700000000000003</v>
+      </c>
+      <c r="P23">
+        <v>0.76200000000000001</v>
+      </c>
+      <c r="Q23">
+        <v>0.76200000000000001</v>
+      </c>
+      <c r="R23" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
     <mergeCell ref="N4:R4"/>
     <mergeCell ref="O5:R5"/>
     <mergeCell ref="B5:E5"/>
@@ -1259,17 +1431,759 @@
     <mergeCell ref="H4:L4"/>
     <mergeCell ref="I5:L5"/>
     <mergeCell ref="I15:L15"/>
+    <mergeCell ref="O15:R15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E80E9AE1-725C-463E-B6B2-6B985631E5DE}">
+  <dimension ref="B2:I43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33:I33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C3" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C4" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" t="s">
+        <v>62</v>
+      </c>
+      <c r="I5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="D6">
+        <v>0.90100000000000002</v>
+      </c>
+      <c r="E6">
+        <v>0.78900000000000003</v>
+      </c>
+      <c r="F6">
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="G6">
+        <v>0.98699999999999999</v>
+      </c>
+      <c r="H6">
+        <v>0.86399999999999999</v>
+      </c>
+      <c r="I6">
+        <v>0.88100000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="D7">
+        <v>0.96199999999999997</v>
+      </c>
+      <c r="E7">
+        <v>0.92</v>
+      </c>
+      <c r="F7">
+        <v>0.93300000000000005</v>
+      </c>
+      <c r="G7">
+        <v>0.98099999999999998</v>
+      </c>
+      <c r="H7">
+        <v>0.95099999999999996</v>
+      </c>
+      <c r="I7">
+        <v>0.95699999999999996</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="D8">
+        <v>0.96199999999999997</v>
+      </c>
+      <c r="E8">
+        <v>0.92</v>
+      </c>
+      <c r="F8">
+        <v>0.92300000000000004</v>
+      </c>
+      <c r="G8">
+        <v>0.98799999999999999</v>
+      </c>
+      <c r="H8">
+        <v>0.95199999999999996</v>
+      </c>
+      <c r="I8">
+        <v>0.95599999999999996</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C11" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" t="s">
+        <v>12</v>
+      </c>
+      <c r="H12" t="s">
+        <v>62</v>
+      </c>
+      <c r="I12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>0.29299999999999998</v>
+      </c>
+      <c r="D13">
+        <v>0.8</v>
+      </c>
+      <c r="E13">
+        <v>0.57799999999999996</v>
+      </c>
+      <c r="F13">
+        <v>0.70699999999999996</v>
+      </c>
+      <c r="G13">
+        <v>0.86299999999999999</v>
+      </c>
+      <c r="H13">
+        <v>0.74</v>
+      </c>
+      <c r="I13">
+        <v>0.78500000000000003</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="D14">
+        <v>0.80600000000000005</v>
+      </c>
+      <c r="E14">
+        <v>0.60699999999999998</v>
+      </c>
+      <c r="F14">
+        <v>0.79500000000000004</v>
+      </c>
+      <c r="G14">
+        <v>0.81799999999999995</v>
+      </c>
+      <c r="H14">
+        <v>0.77100000000000002</v>
+      </c>
+      <c r="I14">
+        <v>0.80700000000000005</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>0.218</v>
+      </c>
+      <c r="D15">
+        <v>0.80400000000000005</v>
+      </c>
+      <c r="E15">
+        <v>0.59599999999999997</v>
+      </c>
+      <c r="F15">
+        <v>0.78200000000000003</v>
+      </c>
+      <c r="G15">
+        <v>0.81799999999999995</v>
+      </c>
+      <c r="H15">
+        <v>0.76300000000000001</v>
+      </c>
+      <c r="I15">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C17" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" t="s">
+        <v>11</v>
+      </c>
+      <c r="G18" t="s">
+        <v>12</v>
+      </c>
+      <c r="H18" t="s">
+        <v>62</v>
+      </c>
+      <c r="I18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="D19">
+        <v>0.97699999999999998</v>
+      </c>
+      <c r="E19">
+        <v>0.95199999999999996</v>
+      </c>
+      <c r="F19">
+        <v>0.97199999999999998</v>
+      </c>
+      <c r="G19">
+        <v>0.98</v>
+      </c>
+      <c r="H19">
+        <v>0.97099999999999997</v>
+      </c>
+      <c r="I19">
+        <v>0.97599999999999998</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D20">
+        <v>0.98799999999999999</v>
+      </c>
+      <c r="E20">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="F20">
+        <v>0.98499999999999999</v>
+      </c>
+      <c r="G20">
+        <v>0.99099999999999999</v>
+      </c>
+      <c r="H20">
+        <v>0.98599999999999999</v>
+      </c>
+      <c r="I20">
+        <v>0.98799999999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D21">
+        <v>0.98799999999999999</v>
+      </c>
+      <c r="E21">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="F21">
+        <v>0.98499999999999999</v>
+      </c>
+      <c r="G21">
+        <v>0.99099999999999999</v>
+      </c>
+      <c r="H21">
+        <v>0.98599999999999999</v>
+      </c>
+      <c r="I21">
+        <v>0.98799999999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C25" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C26" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" t="s">
+        <v>10</v>
+      </c>
+      <c r="F27" t="s">
+        <v>11</v>
+      </c>
+      <c r="G27" t="s">
+        <v>12</v>
+      </c>
+      <c r="H27" t="s">
+        <v>62</v>
+      </c>
+      <c r="I27" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <v>0.127</v>
+      </c>
+      <c r="D28">
+        <v>0.93899999999999995</v>
+      </c>
+      <c r="E28">
+        <v>0.871</v>
+      </c>
+      <c r="F28">
+        <v>0.873</v>
+      </c>
+      <c r="G28">
+        <v>0.98399999999999999</v>
+      </c>
+      <c r="H28">
+        <v>0.92</v>
+      </c>
+      <c r="I28">
+        <v>0.92300000000000004</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>3</v>
+      </c>
+      <c r="C29">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="D29">
+        <v>0.95399999999999996</v>
+      </c>
+      <c r="E29">
+        <v>0.90600000000000003</v>
+      </c>
+      <c r="F29">
+        <v>0.94799999999999995</v>
+      </c>
+      <c r="G29">
+        <v>0.95899999999999996</v>
+      </c>
+      <c r="H29">
+        <v>0.94399999999999995</v>
+      </c>
+      <c r="I29">
+        <v>0.95299999999999996</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="D30">
+        <v>0.96299999999999997</v>
+      </c>
+      <c r="E30">
+        <v>0.92400000000000004</v>
+      </c>
+      <c r="F30">
+        <v>0.93899999999999995</v>
+      </c>
+      <c r="G30">
+        <v>0.98</v>
+      </c>
+      <c r="H30">
+        <v>0.95399999999999996</v>
+      </c>
+      <c r="I30">
+        <v>0.95599999999999996</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C33" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="6"/>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>8</v>
+      </c>
+      <c r="D34" t="s">
+        <v>9</v>
+      </c>
+      <c r="E34" t="s">
+        <v>10</v>
+      </c>
+      <c r="F34" t="s">
+        <v>11</v>
+      </c>
+      <c r="G34" t="s">
+        <v>12</v>
+      </c>
+      <c r="H34" t="s">
+        <v>62</v>
+      </c>
+      <c r="I34" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>1</v>
+      </c>
+      <c r="C35">
+        <v>0.29199999999999998</v>
+      </c>
+      <c r="D35">
+        <v>0.8</v>
+      </c>
+      <c r="E35">
+        <v>0.57899999999999996</v>
+      </c>
+      <c r="F35">
+        <v>0.70799999999999996</v>
+      </c>
+      <c r="G35">
+        <v>0.86299999999999999</v>
+      </c>
+      <c r="H35">
+        <v>0.74199999999999999</v>
+      </c>
+      <c r="I35">
+        <v>0.78500000000000003</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>3</v>
+      </c>
+      <c r="C36">
+        <v>0.20200000000000001</v>
+      </c>
+      <c r="D36">
+        <v>0.81</v>
+      </c>
+      <c r="E36">
+        <v>0.60899999999999999</v>
+      </c>
+      <c r="F36">
+        <v>0.79800000000000004</v>
+      </c>
+      <c r="G36">
+        <v>0.81799999999999995</v>
+      </c>
+      <c r="H36">
+        <v>0.77300000000000002</v>
+      </c>
+      <c r="I36">
+        <v>0.80700000000000005</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37">
+        <v>0.215</v>
+      </c>
+      <c r="D37">
+        <v>0.80400000000000005</v>
+      </c>
+      <c r="E37">
+        <v>0.59699999999999998</v>
+      </c>
+      <c r="F37">
+        <v>0.78500000000000003</v>
+      </c>
+      <c r="G37">
+        <v>0.81699999999999995</v>
+      </c>
+      <c r="H37">
+        <v>0.76500000000000001</v>
+      </c>
+      <c r="I37">
+        <v>0.80100000000000005</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C39" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="6"/>
+      <c r="H39" s="6"/>
+      <c r="I39" s="6"/>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>8</v>
+      </c>
+      <c r="D40" t="s">
+        <v>9</v>
+      </c>
+      <c r="E40" t="s">
+        <v>10</v>
+      </c>
+      <c r="F40" t="s">
+        <v>11</v>
+      </c>
+      <c r="G40" t="s">
+        <v>12</v>
+      </c>
+      <c r="H40" t="s">
+        <v>62</v>
+      </c>
+      <c r="I40" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>1</v>
+      </c>
+      <c r="C41">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="D41">
+        <v>0.97299999999999998</v>
+      </c>
+      <c r="E41">
+        <v>0.94399999999999995</v>
+      </c>
+      <c r="F41">
+        <v>0.96699999999999997</v>
+      </c>
+      <c r="G41">
+        <v>0.97699999999999998</v>
+      </c>
+      <c r="H41">
+        <v>0.96699999999999997</v>
+      </c>
+      <c r="I41">
+        <v>0.97199999999999998</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>3</v>
+      </c>
+      <c r="C42">
+        <v>1.6E-2</v>
+      </c>
+      <c r="D42">
+        <v>0.98799999999999999</v>
+      </c>
+      <c r="E42">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="F42">
+        <v>0.98399999999999999</v>
+      </c>
+      <c r="G42">
+        <v>0.99</v>
+      </c>
+      <c r="H42">
+        <v>0.98499999999999999</v>
+      </c>
+      <c r="I42">
+        <v>0.98699999999999999</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>4</v>
+      </c>
+      <c r="C43">
+        <v>1.6E-2</v>
+      </c>
+      <c r="D43">
+        <v>0.98799999999999999</v>
+      </c>
+      <c r="E43">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="F43">
+        <v>0.98399999999999999</v>
+      </c>
+      <c r="G43">
+        <v>0.99</v>
+      </c>
+      <c r="H43">
+        <v>0.98499999999999999</v>
+      </c>
+      <c r="I43">
+        <v>0.98699999999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="C39:I39"/>
+    <mergeCell ref="C25:I25"/>
+    <mergeCell ref="C26:I26"/>
+    <mergeCell ref="C33:I33"/>
+    <mergeCell ref="C3:I3"/>
+    <mergeCell ref="C4:I4"/>
+    <mergeCell ref="C11:I11"/>
+    <mergeCell ref="C17:I17"/>
+    <mergeCell ref="C2:G2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF879E42-A152-498B-9F7D-3EABAA260A27}">
-  <dimension ref="A3:O25"/>
+  <dimension ref="A2:O51"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView topLeftCell="A2" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1285,27 +2199,35 @@
     <col min="15" max="15" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+    </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="7"/>
-      <c r="K3" s="7" t="s">
+      <c r="I3" s="8"/>
+      <c r="K3" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="L3" s="7"/>
-      <c r="N3" s="7" t="s">
+      <c r="L3" s="8"/>
+      <c r="N3" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="O3" s="7"/>
+      <c r="O3" s="8"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
       <c r="H4" s="2" t="s">
         <v>16</v>
       </c>
@@ -1485,23 +2407,23 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="H12" s="7" t="s">
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="H12" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="I12" s="7"/>
-      <c r="K12" s="7" t="s">
+      <c r="I12" s="8"/>
+      <c r="K12" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="L12" s="7"/>
-      <c r="N12" s="7" t="s">
+      <c r="L12" s="8"/>
+      <c r="N12" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="O12" s="7"/>
+      <c r="O12" s="8"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
@@ -1684,11 +2606,11 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
@@ -1712,7 +2634,9 @@
       <c r="C22" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D22" s="2"/>
+      <c r="D22" s="2">
+        <v>0.56299999999999994</v>
+      </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
@@ -1724,7 +2648,9 @@
       <c r="C23" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D23" s="2"/>
+      <c r="D23" s="2">
+        <v>0.22700000000000001</v>
+      </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
@@ -1736,7 +2662,9 @@
       <c r="C24" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D24" s="2"/>
+      <c r="D24" s="2">
+        <v>0.59399999999999997</v>
+      </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
@@ -1748,10 +2676,248 @@
       <c r="C25" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D25" s="2"/>
+      <c r="D25" s="2">
+        <v>0.46700000000000003</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" s="4"/>
+      <c r="B30" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" s="4"/>
+      <c r="B31" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B32" s="2">
+        <v>0.35599999999999998</v>
+      </c>
+      <c r="C32" s="2">
+        <v>0.45700000000000002</v>
+      </c>
+      <c r="D32" s="2">
+        <v>0.59799999999999998</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B33" s="2">
+        <v>0.127</v>
+      </c>
+      <c r="C33" s="2">
+        <v>0.20899999999999999</v>
+      </c>
+      <c r="D33" s="2">
+        <v>0.35799999999999998</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B34" s="2">
+        <v>0.84</v>
+      </c>
+      <c r="C34" s="2">
+        <v>0.73699999999999999</v>
+      </c>
+      <c r="D34" s="2">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B35" s="2">
+        <v>0.24099999999999999</v>
+      </c>
+      <c r="C35" s="2">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="D35" s="2">
+        <v>0.501</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="4"/>
+      <c r="B38" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="3"/>
+      <c r="B39" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B40" s="2">
+        <v>0.27600000000000002</v>
+      </c>
+      <c r="C40" s="2">
+        <v>0.35499999999999998</v>
+      </c>
+      <c r="D40" s="2">
+        <v>0.89900000000000002</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B41" s="2">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="C41" s="2">
+        <v>0.126</v>
+      </c>
+      <c r="D41" s="2">
+        <v>0.80700000000000005</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B42" s="2">
+        <v>0.90200000000000002</v>
+      </c>
+      <c r="C42" s="2">
+        <v>0.83699999999999997</v>
+      </c>
+      <c r="D42" s="2">
+        <v>0.34300000000000003</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B43" s="2">
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="C43" s="2">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="D43" s="2">
+        <v>0.72699999999999998</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="4"/>
+      <c r="B46" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C46" s="8"/>
+      <c r="D46" s="8"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="4"/>
+      <c r="B47" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B48" s="2">
+        <v>0.36</v>
+      </c>
+      <c r="C48" s="2">
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="D48" s="2">
+        <v>0.439</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B49" s="2">
+        <v>0.13</v>
+      </c>
+      <c r="C49" s="2">
+        <v>0.22600000000000001</v>
+      </c>
+      <c r="D49" s="2">
+        <v>0.24299999999999999</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B50" s="2">
+        <v>0.83499999999999996</v>
+      </c>
+      <c r="C50" s="2">
+        <v>0.71299999999999997</v>
+      </c>
+      <c r="D50" s="2">
+        <v>0.47899999999999998</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B51" s="2">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="C51" s="2">
+        <v>0.377</v>
+      </c>
+      <c r="D51" s="2">
+        <v>0.54300000000000004</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="14">
     <mergeCell ref="N3:O3"/>
     <mergeCell ref="N12:O12"/>
     <mergeCell ref="B12:D12"/>
@@ -1761,6 +2927,11 @@
     <mergeCell ref="H12:I12"/>
     <mergeCell ref="K3:L3"/>
     <mergeCell ref="K12:L12"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="B46:D46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Foram preenchidas as tabelas de resultados e foi adicionado o random forest ao código
</commit_message>
<xml_diff>
--- a/Trabalho_Pratico/Fase_2/Model Comparison.xlsx
+++ b/Trabalho_Pratico/Fase_2/Model Comparison.xlsx
@@ -5,17 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rreis\Desktop\MEIC\2_Semestre\MDLE-23-24\Trabalho_Pratico\Fase_2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ricardo\Github\MDLE-23-24\Trabalho_Pratico\Fase_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7882AD2-5A6E-49EC-A821-91F694E4094F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17BEBC91-00F2-4423-81CF-840DD312F68A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Energy Dataset" sheetId="1" r:id="rId1"/>
     <sheet name="Energy Dataset Models" sheetId="3" r:id="rId2"/>
     <sheet name="Weather Dataset" sheetId="2" r:id="rId3"/>
+    <sheet name="Weather Dataset Models" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="75">
   <si>
     <t>Energy Dataset</t>
   </si>
@@ -246,6 +247,12 @@
   </si>
   <si>
     <t>SEED = 333</t>
+  </si>
+  <si>
+    <t>Gradient Boosted Trees</t>
+  </si>
+  <si>
+    <t>Linear Regression</t>
   </si>
 </sst>
 </file>
@@ -330,7 +337,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -346,12 +353,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -635,7 +649,7 @@
   <dimension ref="A2:R23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:E13"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1441,8 +1455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E80E9AE1-725C-463E-B6B2-6B985631E5DE}">
   <dimension ref="B2:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33:I33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2164,6 +2178,7 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="C2:G2"/>
     <mergeCell ref="C39:I39"/>
     <mergeCell ref="C25:I25"/>
     <mergeCell ref="C26:I26"/>
@@ -2172,7 +2187,6 @@
     <mergeCell ref="C4:I4"/>
     <mergeCell ref="C11:I11"/>
     <mergeCell ref="C17:I17"/>
-    <mergeCell ref="C2:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2182,8 +2196,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF879E42-A152-498B-9F7D-3EABAA260A27}">
   <dimension ref="A2:O51"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D2"/>
+    <sheetView zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2200,34 +2214,34 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="8"/>
-      <c r="K3" s="8" t="s">
+      <c r="I3" s="7"/>
+      <c r="K3" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="L3" s="8"/>
-      <c r="N3" s="8" t="s">
+      <c r="L3" s="7"/>
+      <c r="N3" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="O3" s="8"/>
+      <c r="O3" s="7"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
       <c r="H4" s="2" t="s">
         <v>16</v>
       </c>
@@ -2407,23 +2421,23 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="H12" s="8" t="s">
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="H12" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="I12" s="8"/>
-      <c r="K12" s="8" t="s">
+      <c r="I12" s="7"/>
+      <c r="K12" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="L12" s="8"/>
-      <c r="N12" s="8" t="s">
+      <c r="L12" s="7"/>
+      <c r="N12" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="O12" s="8"/>
+      <c r="O12" s="7"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
@@ -2606,11 +2620,11 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
@@ -2681,20 +2695,20 @@
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="7" t="s">
+      <c r="A28" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
-      <c r="B30" s="8" t="s">
+      <c r="B30" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
@@ -2766,11 +2780,11 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
-      <c r="B38" s="8" t="s">
+      <c r="B38" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C38" s="8"/>
-      <c r="D38" s="8"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="7"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="3"/>
@@ -2842,11 +2856,11 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="4"/>
-      <c r="B46" s="8" t="s">
+      <c r="B46" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C46" s="8"/>
-      <c r="D46" s="8"/>
+      <c r="C46" s="7"/>
+      <c r="D46" s="7"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="4"/>
@@ -2918,6 +2932,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="B46:D46"/>
     <mergeCell ref="N3:O3"/>
     <mergeCell ref="N12:O12"/>
     <mergeCell ref="B12:D12"/>
@@ -2927,11 +2946,363 @@
     <mergeCell ref="H12:I12"/>
     <mergeCell ref="K3:L3"/>
     <mergeCell ref="K12:L12"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A28:D28"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="B46:D46"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C87BA84B-BE3E-4887-8D1B-D7D5677EF7A0}">
+  <dimension ref="A1:E32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="9"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="11">
+        <v>1.5860000000000001</v>
+      </c>
+      <c r="C5" s="11">
+        <v>1.629</v>
+      </c>
+      <c r="D5" s="11">
+        <v>2.3220000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="11">
+        <v>2.516</v>
+      </c>
+      <c r="C6" s="11">
+        <v>2.6539999999999999</v>
+      </c>
+      <c r="D6" s="11">
+        <v>5.3920000000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="11">
+        <v>0.84899999999999998</v>
+      </c>
+      <c r="C7" s="11">
+        <v>0.84</v>
+      </c>
+      <c r="D7" s="11">
+        <v>0.67600000000000005</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="11">
+        <v>1.252</v>
+      </c>
+      <c r="C8" s="11">
+        <v>1.2769999999999999</v>
+      </c>
+      <c r="D8" s="11">
+        <v>1.905</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="9"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="11">
+        <v>2.48</v>
+      </c>
+      <c r="C12" s="11">
+        <v>2.5419999999999998</v>
+      </c>
+      <c r="D12" s="11">
+        <v>3.0939999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="11">
+        <v>6.1509999999999998</v>
+      </c>
+      <c r="C13" s="11">
+        <v>6.46</v>
+      </c>
+      <c r="D13" s="11">
+        <v>9.5709999999999997</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="11">
+        <v>0.63</v>
+      </c>
+      <c r="C14" s="11">
+        <v>0.61099999999999999</v>
+      </c>
+      <c r="D14" s="11">
+        <v>0.42399999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="11">
+        <v>1.9590000000000001</v>
+      </c>
+      <c r="C15" s="11">
+        <v>1.9330000000000001</v>
+      </c>
+      <c r="D15" s="11">
+        <v>2.431</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="9"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="11">
+        <v>1.496</v>
+      </c>
+      <c r="C19" s="11">
+        <v>1.5940000000000001</v>
+      </c>
+      <c r="D19" s="11">
+        <v>2.593</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="11">
+        <v>2.238</v>
+      </c>
+      <c r="C20" s="11">
+        <v>2.5409999999999999</v>
+      </c>
+      <c r="D20" s="11">
+        <v>6.726</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="11">
+        <v>0.86499999999999999</v>
+      </c>
+      <c r="C21" s="11">
+        <v>0.84699999999999998</v>
+      </c>
+      <c r="D21" s="11">
+        <v>0.59499999999999997</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" s="11">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="C22" s="11">
+        <v>1.1779999999999999</v>
+      </c>
+      <c r="D22" s="11">
+        <v>1.988</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E23" s="12"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="13"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E25" s="12"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" s="11">
+        <v>1.0920000000000001</v>
+      </c>
+      <c r="C26" s="11">
+        <v>1.214</v>
+      </c>
+      <c r="D26" s="11">
+        <v>2.6850000000000001</v>
+      </c>
+      <c r="E26" s="12"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" s="11">
+        <v>1.1910000000000001</v>
+      </c>
+      <c r="C27" s="11">
+        <v>1.474</v>
+      </c>
+      <c r="D27" s="11">
+        <v>7.21</v>
+      </c>
+      <c r="E27" s="12"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28" s="11">
+        <v>0.92800000000000005</v>
+      </c>
+      <c r="C28" s="11">
+        <v>0.91100000000000003</v>
+      </c>
+      <c r="D28" s="11">
+        <v>0.56599999999999995</v>
+      </c>
+      <c r="E28" s="12"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29" s="11">
+        <v>0.75700000000000001</v>
+      </c>
+      <c r="C29" s="11">
+        <v>0.85699999999999998</v>
+      </c>
+      <c r="D29" s="11">
+        <v>2.0920000000000001</v>
+      </c>
+      <c r="E29" s="12"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E30" s="12"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E31" s="12"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E32" s="12"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B24:D24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Foi adicionada a seed ao código e foi corrigido o ficheiro excel
</commit_message>
<xml_diff>
--- a/Trabalho_Pratico/Fase_2/Model Comparison.xlsx
+++ b/Trabalho_Pratico/Fase_2/Model Comparison.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ricardo\Github\MDLE-23-24\Trabalho_Pratico\Fase_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17BEBC91-00F2-4423-81CF-840DD312F68A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5BD567C-6FF3-47F0-998B-34D9D076315E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Energy Dataset" sheetId="1" r:id="rId1"/>
     <sheet name="Energy Dataset Models" sheetId="3" r:id="rId2"/>
-    <sheet name="Weather Dataset" sheetId="2" r:id="rId3"/>
-    <sheet name="Weather Dataset Models" sheetId="4" r:id="rId4"/>
+    <sheet name="Weather Dataset Models" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="44">
   <si>
     <t>Energy Dataset</t>
   </si>
@@ -75,9 +74,6 @@
     <t>Com o dataset da Feature Selection</t>
   </si>
   <si>
-    <t>Dataset com Fisher's Ratio</t>
-  </si>
-  <si>
     <t>Conditions</t>
   </si>
   <si>
@@ -114,108 +110,6 @@
     <t>mae</t>
   </si>
   <si>
-    <t>Dataset com Information Gain</t>
-  </si>
-  <si>
-    <t>0.362</t>
-  </si>
-  <si>
-    <t>0.131</t>
-  </si>
-  <si>
-    <t>0.832</t>
-  </si>
-  <si>
-    <t>0.22</t>
-  </si>
-  <si>
-    <t>0.308</t>
-  </si>
-  <si>
-    <t>0.095</t>
-  </si>
-  <si>
-    <t>0.883</t>
-  </si>
-  <si>
-    <t>0.195</t>
-  </si>
-  <si>
-    <t>0.356</t>
-  </si>
-  <si>
-    <t>0.127</t>
-  </si>
-  <si>
-    <t>0.846</t>
-  </si>
-  <si>
-    <t>0.225</t>
-  </si>
-  <si>
-    <t>0.455</t>
-  </si>
-  <si>
-    <t>0.207</t>
-  </si>
-  <si>
-    <t>0.734</t>
-  </si>
-  <si>
-    <t>0.368</t>
-  </si>
-  <si>
-    <t>0.373</t>
-  </si>
-  <si>
-    <t>0.139</t>
-  </si>
-  <si>
-    <t>0.829</t>
-  </si>
-  <si>
-    <t>0.269</t>
-  </si>
-  <si>
-    <t>Dataset com Variance Threshold</t>
-  </si>
-  <si>
-    <t>0.439</t>
-  </si>
-  <si>
-    <t>0.193</t>
-  </si>
-  <si>
-    <t>0.766</t>
-  </si>
-  <si>
-    <t>0.347</t>
-  </si>
-  <si>
-    <t>0.535</t>
-  </si>
-  <si>
-    <t>0.286</t>
-  </si>
-  <si>
-    <t>0.632</t>
-  </si>
-  <si>
-    <t>0.445</t>
-  </si>
-  <si>
-    <t>0.578</t>
-  </si>
-  <si>
-    <t>0.334</t>
-  </si>
-  <si>
-    <t>0.589</t>
-  </si>
-  <si>
-    <t>0.514</t>
-  </si>
-  <si>
     <t>F1 Score</t>
   </si>
   <si>
@@ -234,9 +128,6 @@
     <t>SEED = 1111</t>
   </si>
   <si>
-    <t>SEED = 377</t>
-  </si>
-  <si>
     <t>Random Forest</t>
   </si>
   <si>
@@ -253,6 +144,21 @@
   </si>
   <si>
     <t>Linear Regression</t>
+  </si>
+  <si>
+    <t>Clear</t>
+  </si>
+  <si>
+    <t>Overcast</t>
+  </si>
+  <si>
+    <t>Partially Cloudy</t>
+  </si>
+  <si>
+    <t>Rain, Overcast</t>
+  </si>
+  <si>
+    <t>Rain, Partially Cloudy</t>
   </si>
 </sst>
 </file>
@@ -315,57 +221,54 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right/>
+      <top style="thin">
         <color indexed="64"/>
-      </right>
-      <top/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left/>
+      <right style="thin">
         <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -648,7 +551,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:R23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
@@ -681,47 +584,47 @@
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="H4" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="N4" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="O4" s="6"/>
-      <c r="P4" s="6"/>
-      <c r="Q4" s="6"/>
-      <c r="R4" s="6"/>
+      <c r="A4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="H4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="N4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="4"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="I5" s="6" t="s">
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="I5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="O5" s="6" t="s">
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="O5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="P5" s="6"/>
-      <c r="Q5" s="6"/>
-      <c r="R5" s="6"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="4"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
@@ -968,7 +871,7 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>62</v>
+        <v>27</v>
       </c>
       <c r="B12">
         <v>0.86399999999999999</v>
@@ -983,7 +886,7 @@
         <v>13</v>
       </c>
       <c r="H12" t="s">
-        <v>62</v>
+        <v>27</v>
       </c>
       <c r="I12">
         <v>0.94499999999999995</v>
@@ -998,7 +901,7 @@
         <v>13</v>
       </c>
       <c r="N12" t="s">
-        <v>62</v>
+        <v>27</v>
       </c>
       <c r="O12">
         <v>0.92400000000000004</v>
@@ -1009,7 +912,7 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>63</v>
+        <v>28</v>
       </c>
       <c r="B13">
         <v>0.88100000000000001</v>
@@ -1024,7 +927,7 @@
         <v>13</v>
       </c>
       <c r="H13" t="s">
-        <v>63</v>
+        <v>28</v>
       </c>
       <c r="I13">
         <v>0.95099999999999996</v>
@@ -1039,7 +942,7 @@
         <v>13</v>
       </c>
       <c r="N13" t="s">
-        <v>63</v>
+        <v>28</v>
       </c>
       <c r="O13">
         <v>0.93100000000000005</v>
@@ -1049,24 +952,24 @@
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="I15" s="6" t="s">
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="I15" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="J15" s="6"/>
-      <c r="K15" s="6"/>
-      <c r="L15" s="6"/>
-      <c r="O15" s="6" t="s">
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+      <c r="O15" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="P15" s="6"/>
-      <c r="Q15" s="6"/>
-      <c r="R15" s="6"/>
+      <c r="P15" s="4"/>
+      <c r="Q15" s="4"/>
+      <c r="R15" s="4"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
@@ -1343,7 +1246,7 @@
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>62</v>
+        <v>27</v>
       </c>
       <c r="B22">
         <v>0.80200000000000005</v>
@@ -1358,7 +1261,7 @@
         <v>13</v>
       </c>
       <c r="H22" t="s">
-        <v>62</v>
+        <v>27</v>
       </c>
       <c r="I22">
         <v>0.72599999999999998</v>
@@ -1373,7 +1276,7 @@
         <v>13</v>
       </c>
       <c r="N22" t="s">
-        <v>62</v>
+        <v>27</v>
       </c>
       <c r="O22">
         <v>0.76200000000000001</v>
@@ -1390,7 +1293,7 @@
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>63</v>
+        <v>28</v>
       </c>
       <c r="B23">
         <v>0.83099999999999996</v>
@@ -1405,7 +1308,7 @@
         <v>13</v>
       </c>
       <c r="H23" t="s">
-        <v>63</v>
+        <v>28</v>
       </c>
       <c r="I23">
         <v>0.77600000000000002</v>
@@ -1420,7 +1323,7 @@
         <v>13</v>
       </c>
       <c r="N23" t="s">
-        <v>63</v>
+        <v>28</v>
       </c>
       <c r="O23">
         <v>0.78700000000000003</v>
@@ -1476,33 +1379,33 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C3" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
+      <c r="C3" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C4" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
+      <c r="C4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
@@ -1521,10 +1424,10 @@
         <v>12</v>
       </c>
       <c r="H5" t="s">
-        <v>62</v>
+        <v>27</v>
       </c>
       <c r="I5" t="s">
-        <v>63</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
@@ -1606,15 +1509,15 @@
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C11" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
+      <c r="C11" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
@@ -1633,10 +1536,10 @@
         <v>12</v>
       </c>
       <c r="H12" t="s">
-        <v>62</v>
+        <v>27</v>
       </c>
       <c r="I12" t="s">
-        <v>63</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
@@ -1718,15 +1621,15 @@
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C17" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
+      <c r="C17" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
@@ -1745,10 +1648,10 @@
         <v>12</v>
       </c>
       <c r="H18" t="s">
-        <v>62</v>
+        <v>27</v>
       </c>
       <c r="I18" t="s">
-        <v>63</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
@@ -1830,26 +1733,26 @@
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C25" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
+      <c r="C25" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C26" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="6"/>
+      <c r="C26" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
@@ -1868,10 +1771,10 @@
         <v>12</v>
       </c>
       <c r="H27" t="s">
-        <v>62</v>
+        <v>27</v>
       </c>
       <c r="I27" t="s">
-        <v>63</v>
+        <v>28</v>
       </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.25">
@@ -1953,15 +1856,15 @@
       </c>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C33" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="6"/>
-      <c r="G33" s="6"/>
-      <c r="H33" s="6"/>
-      <c r="I33" s="6"/>
+      <c r="C33" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4"/>
+      <c r="I33" s="4"/>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
@@ -1980,10 +1883,10 @@
         <v>12</v>
       </c>
       <c r="H34" t="s">
-        <v>62</v>
+        <v>27</v>
       </c>
       <c r="I34" t="s">
-        <v>63</v>
+        <v>28</v>
       </c>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.25">
@@ -2065,15 +1968,15 @@
       </c>
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C39" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="D39" s="6"/>
-      <c r="E39" s="6"/>
-      <c r="F39" s="6"/>
-      <c r="G39" s="6"/>
-      <c r="H39" s="6"/>
-      <c r="I39" s="6"/>
+      <c r="C39" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
+      <c r="H39" s="4"/>
+      <c r="I39" s="4"/>
     </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
@@ -2092,10 +1995,10 @@
         <v>12</v>
       </c>
       <c r="H40" t="s">
-        <v>62</v>
+        <v>27</v>
       </c>
       <c r="I40" t="s">
-        <v>63</v>
+        <v>28</v>
       </c>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.25">
@@ -2193,770 +2096,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF879E42-A152-498B-9F7D-3EABAA260A27}">
-  <dimension ref="A2:O51"/>
-  <sheetViews>
-    <sheetView zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" customWidth="1"/>
-    <col min="9" max="9" width="11.5703125" customWidth="1"/>
-    <col min="11" max="11" width="14" customWidth="1"/>
-    <col min="12" max="12" width="12.42578125" customWidth="1"/>
-    <col min="14" max="14" width="13" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="H3" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="I3" s="7"/>
-      <c r="K3" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="L3" s="7"/>
-      <c r="N3" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="O3" s="7"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="H4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H5" s="2">
-        <v>1</v>
-      </c>
-      <c r="I5" s="2">
-        <v>1189</v>
-      </c>
-      <c r="K5" s="2">
-        <v>1</v>
-      </c>
-      <c r="L5" s="2">
-        <v>1146</v>
-      </c>
-      <c r="N5" s="2">
-        <v>1</v>
-      </c>
-      <c r="O5" s="2">
-        <v>1150</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="H6" s="2">
-        <v>2</v>
-      </c>
-      <c r="I6" s="2">
-        <v>278</v>
-      </c>
-      <c r="K6" s="2">
-        <v>2</v>
-      </c>
-      <c r="L6" s="2">
-        <v>297</v>
-      </c>
-      <c r="N6" s="2">
-        <v>2</v>
-      </c>
-      <c r="O6" s="2">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="H7" s="2">
-        <v>3</v>
-      </c>
-      <c r="I7" s="2">
-        <v>3292</v>
-      </c>
-      <c r="K7" s="2">
-        <v>3</v>
-      </c>
-      <c r="L7" s="2">
-        <v>3319</v>
-      </c>
-      <c r="N7" s="2">
-        <v>3</v>
-      </c>
-      <c r="O7" s="2">
-        <v>3326</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="H8" s="2">
-        <v>4</v>
-      </c>
-      <c r="I8" s="2">
-        <v>10</v>
-      </c>
-      <c r="K8" s="2">
-        <v>4</v>
-      </c>
-      <c r="L8" s="2">
-        <v>6</v>
-      </c>
-      <c r="N8" s="2">
-        <v>4</v>
-      </c>
-      <c r="O8" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="H9" s="2">
-        <v>5</v>
-      </c>
-      <c r="I9" s="2">
-        <v>52</v>
-      </c>
-      <c r="K9" s="2">
-        <v>5</v>
-      </c>
-      <c r="L9" s="2">
-        <v>53</v>
-      </c>
-      <c r="N9" s="2">
-        <v>5</v>
-      </c>
-      <c r="O9" s="2">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="H12" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="I12" s="7"/>
-      <c r="K12" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="L12" s="7"/>
-      <c r="N12" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="O12" s="7"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="L13" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="N13" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="O13" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E14" s="5"/>
-      <c r="H14" s="2">
-        <v>1</v>
-      </c>
-      <c r="I14" s="2">
-        <v>580</v>
-      </c>
-      <c r="K14" s="2">
-        <v>1</v>
-      </c>
-      <c r="L14" s="2">
-        <v>623</v>
-      </c>
-      <c r="N14" s="2">
-        <v>1</v>
-      </c>
-      <c r="O14" s="2">
-        <v>619</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="H15" s="2">
-        <v>2</v>
-      </c>
-      <c r="I15" s="2">
-        <v>170</v>
-      </c>
-      <c r="K15" s="2">
-        <v>2</v>
-      </c>
-      <c r="L15" s="2">
-        <v>151</v>
-      </c>
-      <c r="N15" s="2">
-        <v>2</v>
-      </c>
-      <c r="O15" s="2">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="H16" s="2">
-        <v>3</v>
-      </c>
-      <c r="I16" s="2">
-        <v>1698</v>
-      </c>
-      <c r="K16" s="2">
-        <v>3</v>
-      </c>
-      <c r="L16" s="2">
-        <v>1671</v>
-      </c>
-      <c r="N16" s="2">
-        <v>3</v>
-      </c>
-      <c r="O16" s="2">
-        <v>1664</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="H17" s="2">
-        <v>4</v>
-      </c>
-      <c r="I17" s="2">
-        <v>2</v>
-      </c>
-      <c r="K17" s="2">
-        <v>4</v>
-      </c>
-      <c r="L17" s="2">
-        <v>6</v>
-      </c>
-      <c r="N17" s="2">
-        <v>4</v>
-      </c>
-      <c r="O17" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="H18" s="2">
-        <v>5</v>
-      </c>
-      <c r="I18" s="2">
-        <v>24</v>
-      </c>
-      <c r="K18" s="2">
-        <v>5</v>
-      </c>
-      <c r="L18" s="2">
-        <v>23</v>
-      </c>
-      <c r="N18" s="2">
-        <v>5</v>
-      </c>
-      <c r="O18" s="2">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
-      <c r="B20" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-      <c r="B21" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D22" s="2">
-        <v>0.56299999999999994</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D23" s="2">
-        <v>0.22700000000000001</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D24" s="2">
-        <v>0.59399999999999997</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D25" s="2">
-        <v>0.46700000000000003</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" s="4"/>
-      <c r="B30" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" s="4"/>
-      <c r="B31" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B32" s="2">
-        <v>0.35599999999999998</v>
-      </c>
-      <c r="C32" s="2">
-        <v>0.45700000000000002</v>
-      </c>
-      <c r="D32" s="2">
-        <v>0.59799999999999998</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B33" s="2">
-        <v>0.127</v>
-      </c>
-      <c r="C33" s="2">
-        <v>0.20899999999999999</v>
-      </c>
-      <c r="D33" s="2">
-        <v>0.35799999999999998</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B34" s="2">
-        <v>0.84</v>
-      </c>
-      <c r="C34" s="2">
-        <v>0.73699999999999999</v>
-      </c>
-      <c r="D34" s="2">
-        <v>0.55000000000000004</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B35" s="2">
-        <v>0.24099999999999999</v>
-      </c>
-      <c r="C35" s="2">
-        <v>0.38500000000000001</v>
-      </c>
-      <c r="D35" s="2">
-        <v>0.501</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="4"/>
-      <c r="B38" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C38" s="7"/>
-      <c r="D38" s="7"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="3"/>
-      <c r="B39" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B40" s="2">
-        <v>0.27600000000000002</v>
-      </c>
-      <c r="C40" s="2">
-        <v>0.35499999999999998</v>
-      </c>
-      <c r="D40" s="2">
-        <v>0.89900000000000002</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B41" s="2">
-        <v>7.5999999999999998E-2</v>
-      </c>
-      <c r="C41" s="2">
-        <v>0.126</v>
-      </c>
-      <c r="D41" s="2">
-        <v>0.80700000000000005</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B42" s="2">
-        <v>0.90200000000000002</v>
-      </c>
-      <c r="C42" s="2">
-        <v>0.83699999999999997</v>
-      </c>
-      <c r="D42" s="2">
-        <v>0.34300000000000003</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B43" s="2">
-        <v>0.13900000000000001</v>
-      </c>
-      <c r="C43" s="2">
-        <v>0.23100000000000001</v>
-      </c>
-      <c r="D43" s="2">
-        <v>0.72699999999999998</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="4"/>
-      <c r="B46" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C46" s="7"/>
-      <c r="D46" s="7"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="4"/>
-      <c r="B47" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B48" s="2">
-        <v>0.36</v>
-      </c>
-      <c r="C48" s="2">
-        <v>0.47499999999999998</v>
-      </c>
-      <c r="D48" s="2">
-        <v>0.439</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B49" s="2">
-        <v>0.13</v>
-      </c>
-      <c r="C49" s="2">
-        <v>0.22600000000000001</v>
-      </c>
-      <c r="D49" s="2">
-        <v>0.24299999999999999</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B50" s="2">
-        <v>0.83499999999999996</v>
-      </c>
-      <c r="C50" s="2">
-        <v>0.71299999999999997</v>
-      </c>
-      <c r="D50" s="2">
-        <v>0.47899999999999998</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B51" s="2">
-        <v>0.22500000000000001</v>
-      </c>
-      <c r="C51" s="2">
-        <v>0.377</v>
-      </c>
-      <c r="D51" s="2">
-        <v>0.54300000000000004</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A28:D28"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="B46:D46"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="N12:O12"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="K12:L12"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C87BA84B-BE3E-4887-8D1B-D7D5677EF7A0}">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:N29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2964,345 +2108,580 @@
     <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5703125" customWidth="1"/>
-    <col min="6" max="6" width="9.28515625" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.85546875" customWidth="1"/>
+    <col min="6" max="6" width="5.28515625" customWidth="1"/>
+    <col min="7" max="7" width="20" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.28515625" customWidth="1"/>
+    <col min="9" max="9" width="5.42578125" customWidth="1"/>
+    <col min="10" max="10" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.7109375" customWidth="1"/>
+    <col min="12" max="12" width="5" customWidth="1"/>
+    <col min="13" max="13" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.7109375" customWidth="1"/>
+    <col min="15" max="15" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="9"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="11" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B3" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="G3" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="7"/>
+      <c r="J3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="K3" s="7"/>
+      <c r="M3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="N3" s="7"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+      <c r="G4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="3">
+        <v>1.552</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1.6559999999999999</v>
+      </c>
+      <c r="D5" s="3">
+        <v>2.0779999999999998</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H5" s="2">
+        <v>1189</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="K5" s="2">
+        <v>1146</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="N5" s="2">
+        <v>1150</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="11">
-        <v>1.5860000000000001</v>
-      </c>
-      <c r="C5" s="11">
-        <v>1.629</v>
-      </c>
-      <c r="D5" s="11">
-        <v>2.3220000000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+      <c r="B6" s="3">
+        <v>2.41</v>
+      </c>
+      <c r="C6" s="3">
+        <v>2.7410000000000001</v>
+      </c>
+      <c r="D6" s="3">
+        <v>4.3179999999999996</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H6" s="2">
+        <v>278</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="K6" s="2">
+        <v>297</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="N6" s="2">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="11">
-        <v>2.516</v>
-      </c>
-      <c r="C6" s="11">
-        <v>2.6539999999999999</v>
-      </c>
-      <c r="D6" s="11">
-        <v>5.3920000000000003</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+      <c r="B7" s="3">
+        <v>0.85499999999999998</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.83499999999999996</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0.74</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H7" s="2">
+        <v>3292</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="K7" s="2">
+        <v>3319</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="N7" s="2">
+        <v>3326</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="11">
+      <c r="B8" s="3">
+        <v>1.2030000000000001</v>
+      </c>
+      <c r="C8" s="3">
+        <v>1.28</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1.6679999999999999</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H8" s="2">
+        <v>10</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K8" s="2">
+        <v>6</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N8" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G9" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H9" s="2">
+        <v>52</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="K9" s="2">
+        <v>53</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="N9" s="2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B10" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B11" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="3">
+        <v>2.48</v>
+      </c>
+      <c r="C12" s="3">
+        <v>2.5449999999999999</v>
+      </c>
+      <c r="D12" s="3">
+        <v>2.7029999999999998</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H12" s="7"/>
+      <c r="J12" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="K12" s="7"/>
+      <c r="M12" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N12" s="7"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="3">
+        <v>6.1509999999999998</v>
+      </c>
+      <c r="C13" s="3">
+        <v>6.4790000000000001</v>
+      </c>
+      <c r="D13" s="3">
+        <v>7.3040000000000003</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="3">
+        <v>0.63</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0.61</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0.56100000000000005</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H14" s="2">
+        <v>580</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="K14" s="2">
+        <v>623</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="N14" s="2">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="3">
+        <v>1.9590000000000001</v>
+      </c>
+      <c r="C15" s="3">
+        <v>1.9330000000000001</v>
+      </c>
+      <c r="D15" s="3">
+        <v>2.0590000000000002</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H15" s="2">
+        <v>170</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="K15" s="2">
+        <v>151</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="N15" s="2">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G16" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H16" s="2">
+        <v>1698</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="K16" s="2">
+        <v>1671</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="N16" s="2">
+        <v>1664</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B17" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="G17" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H17" s="2">
+        <v>2</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K17" s="2">
+        <v>6</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N17" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B18" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H18" s="2">
+        <v>24</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="K18" s="2">
+        <v>23</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="N18" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="3">
+        <v>1.496</v>
+      </c>
+      <c r="C19" s="3">
+        <v>1.5940000000000001</v>
+      </c>
+      <c r="D19" s="3">
+        <v>2.1619999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="3">
+        <v>2.238</v>
+      </c>
+      <c r="C20" s="3">
+        <v>2.54</v>
+      </c>
+      <c r="D20" s="3">
+        <v>4.6740000000000004</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="3">
+        <v>0.86499999999999999</v>
+      </c>
+      <c r="C21" s="3">
+        <v>0.84699999999999998</v>
+      </c>
+      <c r="D21" s="3">
+        <v>0.71899999999999997</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" s="3">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="C22" s="3">
+        <v>1.1839999999999999</v>
+      </c>
+      <c r="D22" s="3">
+        <v>1.6579999999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B24" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B25" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" s="3">
+        <v>1.0920000000000001</v>
+      </c>
+      <c r="C26" s="3">
+        <v>1.198</v>
+      </c>
+      <c r="D26" s="3">
+        <v>2.1469999999999998</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27" s="3">
+        <v>1.1910000000000001</v>
+      </c>
+      <c r="C27" s="3">
+        <v>1.4350000000000001</v>
+      </c>
+      <c r="D27" s="3">
+        <v>4.6109999999999998</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" s="3">
+        <v>0.92800000000000005</v>
+      </c>
+      <c r="C28" s="3">
+        <v>0.91400000000000003</v>
+      </c>
+      <c r="D28" s="3">
+        <v>0.72299999999999998</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29" s="3">
+        <v>0.75700000000000001</v>
+      </c>
+      <c r="C29" s="3">
         <v>0.84899999999999998</v>
       </c>
-      <c r="C7" s="11">
-        <v>0.84</v>
-      </c>
-      <c r="D7" s="11">
-        <v>0.67600000000000005</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" s="11">
-        <v>1.252</v>
-      </c>
-      <c r="C8" s="11">
-        <v>1.2769999999999999</v>
-      </c>
-      <c r="D8" s="11">
-        <v>1.905</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="9"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" s="11">
-        <v>2.48</v>
-      </c>
-      <c r="C12" s="11">
-        <v>2.5419999999999998</v>
-      </c>
-      <c r="D12" s="11">
-        <v>3.0939999999999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" s="11">
-        <v>6.1509999999999998</v>
-      </c>
-      <c r="C13" s="11">
-        <v>6.46</v>
-      </c>
-      <c r="D13" s="11">
-        <v>9.5709999999999997</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="11">
-        <v>0.63</v>
-      </c>
-      <c r="C14" s="11">
-        <v>0.61099999999999999</v>
-      </c>
-      <c r="D14" s="11">
-        <v>0.42399999999999999</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" s="11">
-        <v>1.9590000000000001</v>
-      </c>
-      <c r="C15" s="11">
-        <v>1.9330000000000001</v>
-      </c>
-      <c r="D15" s="11">
-        <v>2.431</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="9"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="B19" s="11">
-        <v>1.496</v>
-      </c>
-      <c r="C19" s="11">
-        <v>1.5940000000000001</v>
-      </c>
-      <c r="D19" s="11">
-        <v>2.593</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B20" s="11">
-        <v>2.238</v>
-      </c>
-      <c r="C20" s="11">
-        <v>2.5409999999999999</v>
-      </c>
-      <c r="D20" s="11">
-        <v>6.726</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="B21" s="11">
-        <v>0.86499999999999999</v>
-      </c>
-      <c r="C21" s="11">
-        <v>0.84699999999999998</v>
-      </c>
-      <c r="D21" s="11">
-        <v>0.59499999999999997</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="B22" s="11">
-        <v>1.1200000000000001</v>
-      </c>
-      <c r="C22" s="11">
-        <v>1.1779999999999999</v>
-      </c>
-      <c r="D22" s="11">
-        <v>1.988</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E23" s="12"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="13"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C25" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="D25" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="E25" s="12"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="B26" s="11">
-        <v>1.0920000000000001</v>
-      </c>
-      <c r="C26" s="11">
-        <v>1.214</v>
-      </c>
-      <c r="D26" s="11">
-        <v>2.6850000000000001</v>
-      </c>
-      <c r="E26" s="12"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B27" s="11">
-        <v>1.1910000000000001</v>
-      </c>
-      <c r="C27" s="11">
-        <v>1.474</v>
-      </c>
-      <c r="D27" s="11">
-        <v>7.21</v>
-      </c>
-      <c r="E27" s="12"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="B28" s="11">
-        <v>0.92800000000000005</v>
-      </c>
-      <c r="C28" s="11">
-        <v>0.91100000000000003</v>
-      </c>
-      <c r="D28" s="11">
-        <v>0.56599999999999995</v>
-      </c>
-      <c r="E28" s="12"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="B29" s="11">
-        <v>0.75700000000000001</v>
-      </c>
-      <c r="C29" s="11">
-        <v>0.85699999999999998</v>
-      </c>
-      <c r="D29" s="11">
-        <v>2.0920000000000001</v>
-      </c>
-      <c r="E29" s="12"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E30" s="12"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E31" s="12"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E32" s="12"/>
+      <c r="D29" s="3">
+        <v>1.6439999999999999</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="11">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="B10:D10"/>
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="B24:D24"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="M12:N12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>